<commit_message>
updated template from Stephanie
</commit_message>
<xml_diff>
--- a/e8-template.xlsx
+++ b/e8-template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SawSoe\Desktop\frontend\e8document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephanieInfante\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C4756-595D-4861-8EFE-F53C30E84D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F66362E-5B37-45D2-BF48-7A79EAF89E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2580" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{149B6D2C-B18F-46C6-A9A2-8B48A3F23525}"/>
+    <workbookView xWindow="5745" yWindow="4500" windowWidth="34635" windowHeight="15435" activeTab="8" xr2:uid="{149B6D2C-B18F-46C6-A9A2-8B48A3F23525}"/>
   </bookViews>
   <sheets>
-    <sheet name="1-DoesMyAgencyNeedtoComplete" sheetId="13" r:id="rId1"/>
-    <sheet name="2-AboutYourAgency" sheetId="12" r:id="rId2"/>
-    <sheet name="3-WhatToComplete" sheetId="4" r:id="rId3"/>
+    <sheet name="DoesMyAgencyNeedtoComplete" sheetId="13" r:id="rId1"/>
+    <sheet name="AboutYourAgency" sheetId="12" r:id="rId2"/>
+    <sheet name="WhatToComplete" sheetId="4" r:id="rId3"/>
     <sheet name="PR1" sheetId="1" r:id="rId4"/>
     <sheet name="PR2" sheetId="14" r:id="rId5"/>
     <sheet name="PR3" sheetId="23" r:id="rId6"/>
@@ -42,8 +42,8 @@
     <definedName name="policy">[1]Reference!#REF!</definedName>
     <definedName name="policystatement">[1]Reference!#REF!</definedName>
     <definedName name="policystatement1">[1]Reference!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'1-DoesMyAgencyNeedtoComplete'!$A$1:$I$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'2-AboutYourAgency'!$A$2:$C$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AboutYourAgency!$A$2:$C$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">DoesMyAgencyNeedtoComplete!$A$1:$I$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">PolicyR2[#All]</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">PolicyR4[#All]</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">PolicyR5[#All]</definedName>
@@ -2173,7 +2173,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
@@ -2485,13 +2485,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="19" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2500,7 +2497,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2517,22 +2513,22 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -2542,14 +2538,13 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2570,9 +2565,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="4" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2586,11 +2578,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6757,15 +6747,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>30480</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>220980</xdr:colOff>
+          <xdr:colOff>219075</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>106680</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6823,7 +6813,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>25</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -6883,9 +6873,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>171450</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6945,7 +6935,7 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>68580</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7051,7 +7041,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover"/>
@@ -7078,7 +7068,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover"/>
@@ -7109,7 +7099,6 @@
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6164995D-5379-4B4B-AB4D-A1F7140BC99E}" name="PolicyR3e85" displayName="PolicyR3e85" ref="A26:H27" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" headerRowCellStyle="Normal 2" dataCellStyle="20% - Accent2">
-  <autoFilter ref="A26:H27" xr:uid="{6164995D-5379-4B4B-AB4D-A1F7140BC99E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{CE9FC516-AA87-AA47-BBE7-F770B6728414}" name="PR3-E8.5" dataDxfId="58" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{3669DB3C-1E3A-F141-8792-A74B75841706}" name="Disable untrusted Microsoft Office macros_x000a_Macros are increasingly being used to enable the download of malware.  Adversaries can then access sensitive information, so macros should be secured or disabled" dataDxfId="57" dataCellStyle="Normal 2"/>
@@ -7126,7 +7115,6 @@
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{70ECD7F6-D6AC-3240-8218-56049DE4BA7F}" name="PolicyR3e86" displayName="PolicyR3e86" ref="A29:I30" totalsRowShown="0" headerRowDxfId="50" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A29:I30" xr:uid="{70ECD7F6-D6AC-3240-8218-56049DE4BA7F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ABD558FE-5405-D043-B5BB-041AE84D59F0}" name="PR3-E8.6" dataDxfId="49" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{303CAA2D-9921-9647-B254-DC06DB896724}" name="User application hardening_x000a_Flash, Java and web ads are popular ways to deliver malware to infect computers" dataDxfId="48" dataCellStyle="Normal 2"/>
@@ -7144,7 +7132,6 @@
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{1CBC12C9-0E29-CF4D-A38C-72F34E4C71C3}" name="PolicyR3e87" displayName="PolicyR3e87" ref="A32:H36" totalsRowShown="0" headerRowDxfId="40" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A32:H36" xr:uid="{1CBC12C9-0E29-CF4D-A38C-72F34E4C71C3}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B08649A6-9535-7B4B-9424-F2639303533F}" name="PR3-E8.7" dataDxfId="39" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{D48AFAF8-16EA-C845-AF2F-10692860E891}" name="Multi-factor authentication_x000a_Having multiple levels of authentication makes it harder for adversaries to access your information" dataDxfId="38" dataCellStyle="Normal 2"/>
@@ -7161,7 +7148,6 @@
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{DB2CE024-B531-E342-9F15-E0DD01332C25}" name="PolicyR3e88" displayName="PolicyR3e88" ref="A38:I40" totalsRowShown="0" headerRowDxfId="31" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A38:I40" xr:uid="{DB2CE024-B531-E342-9F15-E0DD01332C25}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DA115D66-DA77-C34E-8E5E-B8F3C0C102A3}" name="PR3-E8.8" dataDxfId="30" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{9455DCEF-0621-DE49-A430-2A4CF43CD784}" name="Routine backup of important information_x000a_An organisation can access up to date important information in the event of a security incident" dataDxfId="29" dataCellStyle="Normal 2"/>
@@ -7179,7 +7165,6 @@
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{031FE43E-217C-2649-AC5F-7A44C958A7D1}" name="PolicyR4" displayName="PolicyR4" ref="A1:G4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A1:G4" xr:uid="{031FE43E-217C-2649-AC5F-7A44C958A7D1}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6E1EDF40-70B6-544B-A986-5E60024AA3D5}" name="#" dataDxfId="16" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{5C238449-1F5D-1D47-AADF-BD451FFA350B}" name="Policy Requirements" dataDxfId="15" dataCellStyle="Normal 2"/>
@@ -7195,7 +7180,6 @@
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{958D11D4-E02A-7043-8E35-69B8DE22E019}" name="PolicyR5" displayName="PolicyR5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A1:E2" xr:uid="{958D11D4-E02A-7043-8E35-69B8DE22E019}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E19B852-1D8F-5B41-B909-40400D58B70B}" name="#" dataDxfId="4" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{21CD23DA-3756-6843-894B-9CB4D083C06A}" name="Policy Requirement" dataDxfId="3" dataCellStyle="Normal 2"/>
@@ -7228,7 +7212,6 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF8D1954-0527-4D54-A6C1-7BED95F1568B}" name="PolicyR1" displayName="PolicyR1" ref="A1:I16" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140" tableBorderDxfId="139">
-  <autoFilter ref="A1:I16" xr:uid="{BF8D1954-0527-4D54-A6C1-7BED95F1568B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1D6B8ED-F221-4E0B-871A-CAE3855BB0B1}" name="#" dataDxfId="138" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{1796E134-381D-45F3-B27C-D8F62FA3AA03}" name="Element" dataDxfId="137" dataCellStyle="Normal 2"/>
@@ -7246,7 +7229,6 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2950E7F6-02D7-764D-A273-EA2A6DD44391}" name="PolicyR2" displayName="PolicyR2" ref="A1:G3" totalsRowShown="0" headerRowDxfId="129" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A1:G3" xr:uid="{2950E7F6-02D7-764D-A273-EA2A6DD44391}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FA59F3E7-505F-2F40-BAFE-861E26F2EE8D}" name="#" dataDxfId="128" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{70BCAEC0-68FC-474D-AF86-1C58BB98A5FB}" name="Policy Requirements" dataDxfId="127" dataCellStyle="Normal 2"/>
@@ -7262,7 +7244,6 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{267DBBEC-EBD9-8047-934C-46C6794C5CA2}" name="PolicyR3" displayName="PolicyR3" ref="A1:H6" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
-  <autoFilter ref="A1:H6" xr:uid="{267DBBEC-EBD9-8047-934C-46C6794C5CA2}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EE3C1643-5589-964D-864E-7B73D51F5975}" name="PR3" dataDxfId="119"/>
     <tableColumn id="2" xr3:uid="{EA5294A1-0FD0-C346-AFD4-64D47D37ACBA}" name="Policy Requirements" dataDxfId="118"/>
@@ -7279,7 +7260,6 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B5BAC64C-6737-4744-A0F0-64FF9F317168}" name="PolicyR3e81" displayName="PolicyR3e81" ref="A10:F12" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A10:F12" xr:uid="{B5BAC64C-6737-4744-A0F0-64FF9F317168}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0AD3CA88-D8A3-F74D-A507-4590E23BBBF8}" name="PR3- E8.1" dataDxfId="108" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{56037E7E-0FE2-CD44-A74F-89152016EBDC}" name="Application whitelisting_x000a_Use application whitelisting to help prevent malicious software and other unapproved programs from running " dataDxfId="107" dataCellStyle="Normal 2"/>
@@ -7294,7 +7274,6 @@
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4A653377-3B06-4E4A-B9FE-6F7AFAEF870E}" name="PolicyR3e82" displayName="PolicyR3e82" ref="A14:K16" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A14:K16" xr:uid="{4A653377-3B06-4E4A-B9FE-6F7AFAEF870E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{38A2B7C7-36B5-0248-9C05-1D30EB7012A6}" name="PR3-E8.2" dataDxfId="99" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{36EC25F1-0F27-8F42-AD9D-0FB4BD449E5E}" name="Patch applications _x000a_Patch applications such as PDF readers, Microsoft Office, Java, Flash Player and web browsers" dataDxfId="98" dataCellStyle="Normal 2"/>
@@ -7314,7 +7293,6 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4C910E91-0772-5946-8CF6-491D3F781DD4}" name="PolicyR3e83" displayName="PolicyR3e83" ref="A18:K21" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87" tableBorderDxfId="86" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A18:K21" xr:uid="{4C910E91-0772-5946-8CF6-491D3F781DD4}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B01B4419-95A1-4A4D-A007-B9D68D4BAEEE}" name="PR3- E8.3" dataDxfId="85" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{4084D5B9-3637-E84B-B64B-B744ECD22695}" name="Patch operating systems_x000a_Patch operating system vulnerabilities" dataDxfId="84" dataCellStyle="Normal 2"/>
@@ -7334,7 +7312,6 @@
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{77C3F932-AF6B-2644-9FE3-9CB36F4B1FC3}" name="PolicyR3e84" displayName="PolicyR3e84" ref="A23:K24" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A23:K24" xr:uid="{77C3F932-AF6B-2644-9FE3-9CB36F4B1FC3}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{66306BC1-EBE7-DC49-AD9D-014EF58F50F2}" name="PR3-E8.4" dataDxfId="71" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{D000608A-BE3C-4C43-BACD-CBF6E4DC7FBC}" name="Minimise users with administrative privileges _x000a_The misuse of administrative privileges is a primary method for attackers to spread inside a target enterprise" dataDxfId="70" dataCellStyle="Normal 2"/>
@@ -7655,51 +7632,51 @@
       <selection activeCell="A8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.77734375" style="46"/>
+    <col min="1" max="16384" width="8.7109375" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="159" t="s">
+    <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-    </row>
-    <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+    </row>
+    <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="161" t="s">
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="155" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="156"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="106"/>
       <c r="B4" s="107"/>
       <c r="C4" s="107"/>
@@ -7710,111 +7687,111 @@
       <c r="H4" s="107"/>
       <c r="I4" s="107"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="163" t="s">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="157" t="s">
         <v>305</v>
       </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
-      <c r="F5" s="164"/>
-      <c r="G5" s="164"/>
-      <c r="H5" s="164"/>
-      <c r="I5" s="165"/>
-    </row>
-    <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="156" t="s">
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
+      <c r="H5" s="158"/>
+      <c r="I5" s="159"/>
+    </row>
+    <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="150" t="s">
         <v>309</v>
       </c>
-      <c r="B6" s="157"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
-      <c r="F6" s="157"/>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="158"/>
-    </row>
-    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="170" t="s">
+      <c r="B6" s="151"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="152"/>
+    </row>
+    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="164" t="s">
         <v>306</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="176"/>
-    </row>
-    <row r="8" spans="1:9" ht="64.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="167" t="s">
+      <c r="B7" s="156"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="170"/>
+    </row>
+    <row r="8" spans="1:9" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="168"/>
-      <c r="C8" s="168"/>
-      <c r="D8" s="168"/>
-      <c r="E8" s="168"/>
-      <c r="F8" s="168"/>
-      <c r="G8" s="168"/>
-      <c r="H8" s="168"/>
-      <c r="I8" s="169"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="170" t="s">
+      <c r="B8" s="162"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="162"/>
+      <c r="H8" s="162"/>
+      <c r="I8" s="163"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="164" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="172"/>
-    </row>
-    <row r="10" spans="1:9" s="47" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="173" t="s">
+      <c r="B9" s="165"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="166"/>
+    </row>
+    <row r="10" spans="1:9" s="47" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="167" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="174"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="175"/>
-    </row>
-    <row r="11" spans="1:9" s="47" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="177" t="s">
+      <c r="B10" s="168"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="168"/>
+      <c r="F10" s="168"/>
+      <c r="G10" s="168"/>
+      <c r="H10" s="168"/>
+      <c r="I10" s="169"/>
+    </row>
+    <row r="11" spans="1:9" s="47" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="171" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="178"/>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="178"/>
-      <c r="G11" s="178"/>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="172"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="172"/>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="108" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="109"/>
-      <c r="C12" s="166" t="s">
+      <c r="C12" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="166"/>
-      <c r="E12" s="166"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="166"/>
-      <c r="H12" s="166"/>
-      <c r="I12" s="166"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="160"/>
+      <c r="G12" s="160"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7854,19 +7831,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="181" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="175" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -7887,15 +7864,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>30480</xdr:colOff>
+                <xdr:colOff>28575</xdr:colOff>
                 <xdr:row>6</xdr:row>
-                <xdr:rowOff>30480</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>9</xdr:col>
-                <xdr:colOff>220980</xdr:colOff>
+                <xdr:colOff>219075</xdr:colOff>
                 <xdr:row>28</xdr:row>
-                <xdr:rowOff>106680</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7920,24 +7897,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="181" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="175" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -7965,7 +7942,7 @@
               </from>
               <to>
                 <xdr:col>8</xdr:col>
-                <xdr:colOff>68580</xdr:colOff>
+                <xdr:colOff>66675</xdr:colOff>
                 <xdr:row>25</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </to>
@@ -7992,24 +7969,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="181" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="175" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -8037,9 +8014,9 @@
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>167640</xdr:colOff>
+                <xdr:colOff>171450</xdr:colOff>
                 <xdr:row>21</xdr:row>
-                <xdr:rowOff>15240</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -8064,24 +8041,24 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="181" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="175" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -8111,7 +8088,7 @@
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>495300</xdr:colOff>
                 <xdr:row>21</xdr:row>
-                <xdr:rowOff>68580</xdr:rowOff>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -8136,22 +8113,22 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5546875" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="154" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="149" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>363</v>
       </c>
@@ -8177,19 +8154,19 @@
       <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="181" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="175" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>259</v>
       </c>
@@ -8244,24 +8221,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>292</v>
       </c>
@@ -8284,143 +8261,143 @@
       <selection activeCell="A21" sqref="A21:I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="21.21875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="9" width="21.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="187" t="s">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="181" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="193" t="s">
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="187" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="193"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
-      <c r="I2" s="193"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="193" t="s">
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="187" t="s">
         <v>269</v>
       </c>
-      <c r="B3" s="193"/>
-      <c r="C3" s="193"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="193"/>
-      <c r="I3" s="193"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="193" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="187" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="193"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="193" t="s">
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="187" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="193"/>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="193"/>
-      <c r="I5" s="193"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="195" t="s">
+      <c r="B5" s="187"/>
+      <c r="C5" s="187"/>
+      <c r="D5" s="187"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="187"/>
+      <c r="G5" s="187"/>
+      <c r="H5" s="187"/>
+      <c r="I5" s="187"/>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="189" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="196"/>
-      <c r="C6" s="196"/>
-      <c r="D6" s="197"/>
+      <c r="B6" s="190"/>
+      <c r="C6" s="190"/>
+      <c r="D6" s="191"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="198"/>
-      <c r="G6" s="199"/>
-      <c r="H6" s="199"/>
-      <c r="I6" s="200"/>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="187" t="s">
+      <c r="F6" s="192"/>
+      <c r="G6" s="193"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="194"/>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="181" t="s">
         <v>272</v>
       </c>
-      <c r="B7" s="187"/>
-      <c r="C7" s="187"/>
-      <c r="D7" s="187"/>
-      <c r="E7" s="187"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="187"/>
-      <c r="H7" s="187"/>
-      <c r="I7" s="187"/>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="193" t="s">
+      <c r="B7" s="181"/>
+      <c r="C7" s="181"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="187" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="193"/>
-      <c r="C8" s="193"/>
-      <c r="D8" s="193"/>
-      <c r="E8" s="193"/>
-      <c r="F8" s="193"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="193"/>
-      <c r="I8" s="193"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="187" t="s">
+      <c r="B8" s="187"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="187"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="187"/>
+      <c r="I8" s="187"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="181" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="187"/>
-      <c r="C9" s="187"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="187"/>
-      <c r="F9" s="187"/>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
-      <c r="I9" s="187"/>
-    </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="185" t="s">
+      <c r="B9" s="181"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="179" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="186"/>
-      <c r="C10" s="186"/>
-      <c r="D10" s="186"/>
-      <c r="E10" s="186"/>
-      <c r="F10" s="186"/>
-      <c r="G10" s="186"/>
-      <c r="H10" s="186"/>
-      <c r="I10" s="186"/>
-    </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="180"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="180"/>
+      <c r="F10" s="180"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="180"/>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -8431,46 +8408,46 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="187" t="s">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="181" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="187"/>
-      <c r="C12" s="187"/>
-      <c r="D12" s="187"/>
-      <c r="E12" s="187"/>
-      <c r="F12" s="187"/>
-      <c r="G12" s="187"/>
-      <c r="H12" s="187"/>
-      <c r="I12" s="187"/>
-    </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="184" t="s">
+      <c r="B12" s="181"/>
+      <c r="C12" s="181"/>
+      <c r="D12" s="181"/>
+      <c r="E12" s="181"/>
+      <c r="F12" s="181"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="181"/>
+      <c r="I12" s="181"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="178" t="s">
         <v>277</v>
       </c>
-      <c r="B13" s="184"/>
-      <c r="C13" s="184"/>
-      <c r="D13" s="184"/>
-      <c r="E13" s="184"/>
-      <c r="F13" s="184"/>
-      <c r="G13" s="184"/>
-      <c r="H13" s="184"/>
-      <c r="I13" s="184"/>
-    </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="185" t="s">
+      <c r="B13" s="178"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="178"/>
+      <c r="F13" s="178"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="178"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="179" t="s">
         <v>278</v>
       </c>
-      <c r="B14" s="186"/>
-      <c r="C14" s="186"/>
-      <c r="D14" s="186"/>
-      <c r="E14" s="186"/>
-      <c r="F14" s="186"/>
-      <c r="G14" s="186"/>
-      <c r="H14" s="186"/>
-      <c r="I14" s="186"/>
-    </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="180"/>
+      <c r="C14" s="180"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -8481,141 +8458,141 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="187" t="s">
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="181" t="s">
         <v>279</v>
       </c>
-      <c r="B16" s="187"/>
-      <c r="C16" s="187"/>
-      <c r="D16" s="187"/>
-      <c r="E16" s="187"/>
-      <c r="F16" s="187"/>
-      <c r="G16" s="187"/>
-      <c r="H16" s="187"/>
-      <c r="I16" s="187"/>
-    </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="188" t="s">
+      <c r="B16" s="181"/>
+      <c r="C16" s="181"/>
+      <c r="D16" s="181"/>
+      <c r="E16" s="181"/>
+      <c r="F16" s="181"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="181"/>
+      <c r="I16" s="181"/>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="182" t="s">
         <v>280</v>
       </c>
-      <c r="B17" s="188"/>
-      <c r="C17" s="188"/>
-      <c r="D17" s="188"/>
-      <c r="E17" s="188"/>
-      <c r="F17" s="188"/>
-      <c r="G17" s="188"/>
-      <c r="H17" s="188"/>
-      <c r="I17" s="188"/>
-    </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="189" t="s">
+      <c r="B17" s="182"/>
+      <c r="C17" s="182"/>
+      <c r="D17" s="182"/>
+      <c r="E17" s="182"/>
+      <c r="F17" s="182"/>
+      <c r="G17" s="182"/>
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="183" t="s">
         <v>281</v>
       </c>
-      <c r="B18" s="190"/>
-      <c r="C18" s="190"/>
-      <c r="D18" s="190"/>
-      <c r="E18" s="190"/>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
-      <c r="H18" s="190"/>
-      <c r="I18" s="190"/>
-    </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="191" t="s">
+      <c r="B18" s="184"/>
+      <c r="C18" s="184"/>
+      <c r="D18" s="184"/>
+      <c r="E18" s="184"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="184"/>
+      <c r="H18" s="184"/>
+      <c r="I18" s="184"/>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="185" t="s">
         <v>282</v>
       </c>
-      <c r="B19" s="191"/>
-      <c r="C19" s="191"/>
-      <c r="D19" s="191"/>
-      <c r="E19" s="191"/>
-      <c r="F19" s="191"/>
-      <c r="G19" s="191"/>
-      <c r="H19" s="191"/>
-      <c r="I19" s="191"/>
-    </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="192" t="s">
+      <c r="B19" s="185"/>
+      <c r="C19" s="185"/>
+      <c r="D19" s="185"/>
+      <c r="E19" s="185"/>
+      <c r="F19" s="185"/>
+      <c r="G19" s="185"/>
+      <c r="H19" s="185"/>
+      <c r="I19" s="185"/>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="192"/>
-      <c r="C20" s="192"/>
-      <c r="D20" s="192"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-    </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="193" t="s">
+      <c r="B20" s="186"/>
+      <c r="C20" s="186"/>
+      <c r="D20" s="186"/>
+      <c r="E20" s="186"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="186"/>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="187" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="193"/>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="193"/>
-    </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="187" t="s">
+      <c r="B21" s="187"/>
+      <c r="C21" s="187"/>
+      <c r="D21" s="187"/>
+      <c r="E21" s="187"/>
+      <c r="F21" s="187"/>
+      <c r="G21" s="187"/>
+      <c r="H21" s="187"/>
+      <c r="I21" s="187"/>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="181" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="187"/>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187"/>
-      <c r="E22" s="187"/>
-      <c r="F22" s="187"/>
-      <c r="G22" s="187"/>
-      <c r="H22" s="187"/>
-      <c r="I22" s="187"/>
-    </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="194" t="s">
+      <c r="B22" s="181"/>
+      <c r="C22" s="181"/>
+      <c r="D22" s="181"/>
+      <c r="E22" s="181"/>
+      <c r="F22" s="181"/>
+      <c r="G22" s="181"/>
+      <c r="H22" s="181"/>
+      <c r="I22" s="181"/>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="188" t="s">
         <v>286</v>
       </c>
-      <c r="B23" s="194"/>
-      <c r="C23" s="194"/>
-      <c r="D23" s="194"/>
-      <c r="E23" s="194"/>
-      <c r="F23" s="194"/>
-      <c r="G23" s="194"/>
-      <c r="H23" s="194"/>
-      <c r="I23" s="194"/>
-    </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="187" t="s">
+      <c r="B23" s="188"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="181" t="s">
         <v>287</v>
       </c>
-      <c r="B24" s="187"/>
-      <c r="C24" s="187"/>
-      <c r="D24" s="187"/>
-      <c r="E24" s="187"/>
-      <c r="F24" s="187"/>
-      <c r="G24" s="187"/>
-      <c r="H24" s="187"/>
-      <c r="I24" s="187"/>
-    </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="182" t="s">
+      <c r="B24" s="181"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="176" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="183"/>
-      <c r="E25" s="183"/>
-      <c r="F25" s="183"/>
-      <c r="G25" s="183"/>
-      <c r="H25" s="183"/>
-      <c r="I25" s="183"/>
-    </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" ht="7.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="177"/>
+      <c r="C25" s="177"/>
+      <c r="D25" s="177"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="177"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="177"/>
+      <c r="I25" s="177"/>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -8675,26 +8652,26 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="52.21875" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+    <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="122" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="125" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="123" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="25" t="s">
@@ -8702,106 +8679,104 @@
       </c>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="126" t="s">
+    <row r="4" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="124" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="123"/>
-    </row>
-    <row r="5" spans="1:3" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="127" t="s">
+      <c r="C4" s="121"/>
+    </row>
+    <row r="5" spans="1:3" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="125" t="s">
         <v>310</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="132" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="125" t="s">
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="123" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="C6" s="135" t="s">
+      <c r="C6" s="133" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="128" t="s">
+    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="126" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="C7" s="136"/>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="129" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="127" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="26">
         <v>468463789</v>
       </c>
-      <c r="C8" s="123"/>
-    </row>
-    <row r="9" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
+      <c r="C8" s="121"/>
+    </row>
+    <row r="9" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="128"/>
       <c r="B9" s="111"/>
-      <c r="C9" s="136"/>
-    </row>
-    <row r="10" spans="1:3" ht="78.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="130" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="128" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="21">
         <v>0</v>
       </c>
-      <c r="C10" s="132" t="s">
+      <c r="C10" s="130" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="131" t="s">
+    <row r="11" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="129" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="29">
         <v>0</v>
       </c>
-      <c r="C11" s="137" t="s">
+      <c r="C11" s="134" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="132" t="s">
+    <row r="12" spans="1:3" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="130" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="138"/>
-    </row>
-    <row r="13" spans="1:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="133"/>
+      <c r="C12" s="135"/>
+    </row>
+    <row r="13" spans="1:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="131"/>
       <c r="B13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="139"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="140" t="s">
+      <c r="C13" s="136"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="141" t="s">
+      <c r="B14" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="142"/>
+      <c r="C14" s="139"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8827,22 +8802,22 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.21875" style="81" customWidth="1"/>
-    <col min="2" max="6" width="28.77734375" style="81" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" style="81" customWidth="1"/>
-    <col min="8" max="8" width="28.77734375" style="81" customWidth="1"/>
-    <col min="9" max="9" width="55.21875" style="81" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="81" customWidth="1"/>
+    <col min="2" max="6" width="28.7109375" style="81" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="81" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="81" customWidth="1"/>
+    <col min="9" max="9" width="55.28515625" style="81" customWidth="1"/>
     <col min="10" max="10" width="0" style="81" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.77734375" style="81"/>
+    <col min="11" max="16384" width="8.7109375" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="103" t="s">
         <v>22</v>
       </c>
@@ -8874,7 +8849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="206.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>307</v>
       </c>
@@ -8906,7 +8881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="191.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>362</v>
       </c>
@@ -8938,7 +8913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="199.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="199.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>308</v>
       </c>
@@ -8988,23 +8963,23 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="81"/>
-    <col min="2" max="2" width="21.21875" style="81" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="81"/>
+    <col min="2" max="2" width="21.28515625" style="81" customWidth="1"/>
     <col min="3" max="3" width="33" style="81" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" style="81" customWidth="1"/>
-    <col min="5" max="6" width="51.77734375" style="81" customWidth="1"/>
-    <col min="7" max="7" width="33.21875" style="81" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" style="81" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="81" customWidth="1"/>
+    <col min="5" max="6" width="51.7109375" style="81" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="81" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="81" customWidth="1"/>
     <col min="9" max="9" width="17" style="81" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="81"/>
+    <col min="10" max="16384" width="8.7109375" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="102" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
         <v>46</v>
       </c>
@@ -9033,7 +9008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="102" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
         <v>53</v>
       </c>
@@ -9054,7 +9029,7 @@
       </c>
       <c r="I2" s="112"/>
     </row>
-    <row r="3" spans="1:9" ht="266.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="266.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="82" t="s">
         <v>56</v>
       </c>
@@ -9074,14 +9049,14 @@
         <v>326</v>
       </c>
       <c r="G3" s="86"/>
-      <c r="H3" s="144" t="s">
+      <c r="H3" s="141" t="s">
         <v>339</v>
       </c>
       <c r="I3" s="59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="82" t="s">
         <v>62</v>
       </c>
@@ -9106,7 +9081,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="345" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="345" x14ac:dyDescent="0.25">
       <c r="A5" s="82" t="s">
         <v>66</v>
       </c>
@@ -9122,14 +9097,14 @@
       <c r="E5" s="85"/>
       <c r="F5" s="85"/>
       <c r="G5" s="86"/>
-      <c r="H5" s="144" t="s">
+      <c r="H5" s="141" t="s">
         <v>339</v>
       </c>
       <c r="I5" s="59" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="195" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" s="82" t="s">
         <v>70</v>
       </c>
@@ -9145,14 +9120,14 @@
       <c r="E6" s="85"/>
       <c r="F6" s="85"/>
       <c r="G6" s="86"/>
-      <c r="H6" s="144" t="s">
+      <c r="H6" s="141" t="s">
         <v>339</v>
       </c>
       <c r="I6" s="59" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="87" t="s">
         <v>74</v>
       </c>
@@ -9175,7 +9150,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="87" t="s">
         <v>80</v>
       </c>
@@ -9191,14 +9166,14 @@
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
       <c r="G8" s="86"/>
-      <c r="H8" s="146" t="s">
+      <c r="H8" s="143" t="s">
         <v>341</v>
       </c>
       <c r="I8" s="59" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="87" t="s">
         <v>84</v>
       </c>
@@ -9214,14 +9189,14 @@
       <c r="E9" s="85"/>
       <c r="F9" s="85"/>
       <c r="G9" s="86"/>
-      <c r="H9" s="146" t="s">
+      <c r="H9" s="143" t="s">
         <v>341</v>
       </c>
       <c r="I9" s="59" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="87" t="s">
         <v>88</v>
       </c>
@@ -9242,7 +9217,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="87" t="s">
         <v>93</v>
       </c>
@@ -9263,7 +9238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="87" t="s">
         <v>97</v>
       </c>
@@ -9284,7 +9259,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="87" t="s">
         <v>101</v>
       </c>
@@ -9300,14 +9275,14 @@
       <c r="E13" s="85"/>
       <c r="F13" s="85"/>
       <c r="G13" s="86"/>
-      <c r="H13" s="145" t="s">
+      <c r="H13" s="142" t="s">
         <v>340</v>
       </c>
       <c r="I13" s="59" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="87" t="s">
         <v>105</v>
       </c>
@@ -9323,14 +9298,14 @@
       <c r="E14" s="85"/>
       <c r="F14" s="85"/>
       <c r="G14" s="86"/>
-      <c r="H14" s="145" t="s">
+      <c r="H14" s="142" t="s">
         <v>340</v>
       </c>
       <c r="I14" s="59" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="87" t="s">
         <v>109</v>
       </c>
@@ -9351,7 +9326,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="92" t="s">
         <v>114</v>
       </c>
@@ -9404,21 +9379,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="75"/>
-    <col min="2" max="3" width="53.77734375" style="75" customWidth="1"/>
-    <col min="4" max="4" width="37.21875" style="75" customWidth="1"/>
-    <col min="5" max="5" width="32.21875" style="75" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="75"/>
+    <col min="2" max="3" width="53.7109375" style="75" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="75" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="75" customWidth="1"/>
     <col min="6" max="6" width="28" style="75" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" style="75" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="75"/>
+    <col min="7" max="7" width="24.28515625" style="75" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>46</v>
       </c>
@@ -9441,7 +9416,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
         <v>118</v>
       </c>
@@ -9458,7 +9433,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="231" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="231" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>119</v>
       </c>
@@ -9468,10 +9443,10 @@
       <c r="C3" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="120" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="122" t="s">
+      <c r="E3" s="120" t="s">
         <v>356</v>
       </c>
       <c r="F3" s="77"/>
@@ -9479,7 +9454,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="87"/>
       <c r="B8" s="88"/>
       <c r="C8" s="83"/>
@@ -9510,27 +9485,27 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="E29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I38" sqref="E38:I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="50" customWidth="1"/>
-    <col min="2" max="2" width="40.21875" style="50" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="50" customWidth="1"/>
     <col min="3" max="3" width="32" style="50" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" style="50" customWidth="1"/>
-    <col min="5" max="5" width="64.77734375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="85.77734375" style="50" customWidth="1"/>
-    <col min="7" max="7" width="66.21875" style="50" customWidth="1"/>
-    <col min="8" max="8" width="85.77734375" style="48" customWidth="1"/>
-    <col min="9" max="9" width="81.21875" style="50" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" style="50" customWidth="1"/>
+    <col min="5" max="5" width="64.7109375" style="50" customWidth="1"/>
+    <col min="6" max="6" width="85.7109375" style="50" customWidth="1"/>
+    <col min="7" max="7" width="66.28515625" style="50" customWidth="1"/>
+    <col min="8" max="8" width="85.7109375" style="48" customWidth="1"/>
+    <col min="9" max="9" width="81.28515625" style="50" customWidth="1"/>
     <col min="10" max="10" width="14" style="50" customWidth="1"/>
     <col min="11" max="11" width="12" style="50" customWidth="1"/>
-    <col min="12" max="16384" width="10.77734375" style="50"/>
+    <col min="12" max="16384" width="10.7109375" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="48" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="48" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
         <v>122</v>
       </c>
@@ -9556,7 +9531,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="48" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="48" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="87" t="s">
         <v>122</v>
       </c>
@@ -9574,7 +9549,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="271.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="271.14999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="71" t="s">
         <v>122</v>
       </c>
@@ -9584,7 +9559,6 @@
       <c r="C3" s="101" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="153"/>
       <c r="E3" s="48"/>
       <c r="F3" s="48" t="s">
         <v>359</v>
@@ -9592,7 +9566,7 @@
       <c r="G3" s="73"/>
       <c r="H3" s="73"/>
     </row>
-    <row r="4" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
         <v>126</v>
       </c>
@@ -9613,7 +9587,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
         <v>129</v>
       </c>
@@ -9628,7 +9602,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="61.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
         <v>132</v>
       </c>
@@ -9643,7 +9617,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="110"/>
       <c r="B7" s="110"/>
       <c r="C7" s="110"/>
@@ -9653,11 +9627,11 @@
       <c r="G7" s="110"/>
       <c r="H7" s="110"/>
     </row>
-    <row r="8" spans="1:11" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="148" t="s">
         <v>358</v>
       </c>
       <c r="C8" s="48" t="s">
@@ -9669,7 +9643,7 @@
       <c r="E8" s="48"/>
       <c r="H8" s="50"/>
     </row>
-    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="73"/>
       <c r="B9" s="105"/>
       <c r="C9" s="48"/>
@@ -9677,7 +9651,7 @@
       <c r="E9" s="12"/>
       <c r="H9" s="50"/>
     </row>
-    <row r="10" spans="1:11" ht="107.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="107.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>136</v>
       </c>
@@ -9699,7 +9673,7 @@
       <c r="G10" s="53"/>
       <c r="H10" s="53"/>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
         <v>142</v>
       </c>
@@ -9718,7 +9692,7 @@
       </c>
       <c r="H11" s="50"/>
     </row>
-    <row r="12" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>144</v>
       </c>
@@ -9737,7 +9711,7 @@
       </c>
       <c r="H12" s="50"/>
     </row>
-    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
@@ -9746,7 +9720,7 @@
       <c r="F13" s="56"/>
       <c r="H13" s="50"/>
     </row>
-    <row r="14" spans="1:11" ht="95.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="95.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>146</v>
       </c>
@@ -9781,7 +9755,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="240" x14ac:dyDescent="0.2">
       <c r="A15" s="54" t="s">
         <v>157</v>
       </c>
@@ -9808,7 +9782,7 @@
       <c r="J15" s="59"/>
       <c r="K15" s="59"/>
     </row>
-    <row r="16" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="225" x14ac:dyDescent="0.2">
       <c r="A16" s="54" t="s">
         <v>160</v>
       </c>
@@ -9835,7 +9809,7 @@
       <c r="J16" s="59"/>
       <c r="K16" s="59"/>
     </row>
-    <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="60"/>
       <c r="B17" s="55"/>
       <c r="C17" s="55"/>
@@ -9848,7 +9822,7 @@
       <c r="J17" s="59"/>
       <c r="K17" s="59"/>
     </row>
-    <row r="18" spans="1:11" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="61" t="s">
         <v>163</v>
       </c>
@@ -9883,7 +9857,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="165" x14ac:dyDescent="0.2">
       <c r="A19" s="62" t="s">
         <v>168</v>
       </c>
@@ -9910,7 +9884,7 @@
       <c r="J19" s="59"/>
       <c r="K19" s="59"/>
     </row>
-    <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.2">
       <c r="A20" s="62" t="s">
         <v>171</v>
       </c>
@@ -9937,7 +9911,7 @@
       <c r="J20" s="59"/>
       <c r="K20" s="59"/>
     </row>
-    <row r="21" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="165" x14ac:dyDescent="0.2">
       <c r="A21" s="63" t="s">
         <v>174</v>
       </c>
@@ -9964,7 +9938,7 @@
       <c r="J21" s="59"/>
       <c r="K21" s="59"/>
     </row>
-    <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="64"/>
       <c r="B22" s="55"/>
       <c r="C22" s="55"/>
@@ -9977,7 +9951,7 @@
       <c r="J22" s="59"/>
       <c r="K22" s="59"/>
     </row>
-    <row r="23" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="61" t="s">
         <v>176</v>
       </c>
@@ -10012,7 +9986,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="78.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="63" t="s">
         <v>185</v>
       </c>
@@ -10033,7 +10007,7 @@
       <c r="J24" s="59"/>
       <c r="K24" s="59"/>
     </row>
-    <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="60"/>
       <c r="B25" s="55"/>
       <c r="C25" s="55"/>
@@ -10046,7 +10020,7 @@
       <c r="J25" s="59"/>
       <c r="K25" s="59"/>
     </row>
-    <row r="26" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
         <v>188</v>
       </c>
@@ -10072,12 +10046,12 @@
         <v>183</v>
       </c>
       <c r="I26" s="53"/>
-      <c r="J26" s="180" t="s">
+      <c r="J26" s="174" t="s">
         <v>155</v>
       </c>
-      <c r="K26" s="180"/>
-    </row>
-    <row r="27" spans="1:11" ht="91.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="174"/>
+    </row>
+    <row r="27" spans="1:11" ht="91.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54" t="s">
         <v>192</v>
       </c>
@@ -10099,10 +10073,10 @@
       </c>
       <c r="H27" s="56"/>
       <c r="I27" s="53"/>
-      <c r="J27" s="179"/>
-      <c r="K27" s="179"/>
-    </row>
-    <row r="28" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="173"/>
+      <c r="K27" s="173"/>
+    </row>
+    <row r="28" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="60"/>
       <c r="B28" s="55"/>
       <c r="C28" s="55"/>
@@ -10115,7 +10089,7 @@
       <c r="J28" s="59"/>
       <c r="K28" s="59"/>
     </row>
-    <row r="29" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="51" t="s">
         <v>196</v>
       </c>
@@ -10144,7 +10118,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
         <v>203</v>
       </c>
@@ -10167,7 +10141,7 @@
       <c r="H30" s="68"/>
       <c r="I30" s="59"/>
     </row>
-    <row r="31" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="60"/>
       <c r="B31" s="55"/>
       <c r="C31" s="55"/>
@@ -10180,7 +10154,7 @@
       <c r="J31" s="59"/>
       <c r="K31" s="59"/>
     </row>
-    <row r="32" spans="1:11" ht="98.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="98.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="51" t="s">
         <v>206</v>
       </c>
@@ -10196,7 +10170,7 @@
       <c r="E32" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F32" s="143" t="s">
+      <c r="F32" s="140" t="s">
         <v>336</v>
       </c>
       <c r="G32" s="52" t="s">
@@ -10207,7 +10181,7 @@
       </c>
       <c r="I32" s="52"/>
     </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="54" t="s">
         <v>211</v>
       </c>
@@ -10230,7 +10204,7 @@
       <c r="H33" s="70"/>
       <c r="I33" s="70"/>
     </row>
-    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="54" t="s">
         <v>214</v>
       </c>
@@ -10253,7 +10227,7 @@
       <c r="H34" s="70"/>
       <c r="I34" s="70"/>
     </row>
-    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A35" s="54" t="s">
         <v>217</v>
       </c>
@@ -10276,7 +10250,7 @@
       <c r="H35" s="70"/>
       <c r="I35" s="70"/>
     </row>
-    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A36" s="54" t="s">
         <v>220</v>
       </c>
@@ -10299,7 +10273,7 @@
       <c r="H36" s="70"/>
       <c r="I36" s="70"/>
     </row>
-    <row r="37" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="60"/>
       <c r="B37" s="55"/>
       <c r="C37" s="55"/>
@@ -10312,7 +10286,7 @@
       <c r="J37" s="59"/>
       <c r="K37" s="59"/>
     </row>
-    <row r="38" spans="1:11" ht="109.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="109.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="51" t="s">
         <v>223</v>
       </c>
@@ -10341,7 +10315,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="54" t="s">
         <v>229</v>
       </c>
@@ -10364,7 +10338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="54" t="s">
         <v>232</v>
       </c>
@@ -10426,21 +10400,21 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="42"/>
-    <col min="2" max="3" width="51.21875" style="42" customWidth="1"/>
-    <col min="4" max="4" width="45.77734375" style="42" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="42"/>
+    <col min="2" max="3" width="51.28515625" style="42" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="42" customWidth="1"/>
     <col min="5" max="5" width="45" style="42" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" style="42" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" style="42" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="42"/>
+    <col min="6" max="6" width="29.28515625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="42" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>46</v>
       </c>
@@ -10463,7 +10437,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="87" t="s">
         <v>330</v>
       </c>
@@ -10480,7 +10454,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="337.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="337.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>235</v>
       </c>
@@ -10499,14 +10473,14 @@
       <c r="F3" s="44"/>
       <c r="G3" s="115"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="116"/>
       <c r="B4" s="117"/>
-      <c r="C4" s="118"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="117"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="121"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="115"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10530,19 +10504,19 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="30"/>
-    <col min="2" max="3" width="70.77734375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="44.21875" style="30" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="30"/>
+    <col min="1" max="1" width="8.7109375" style="30"/>
+    <col min="2" max="3" width="70.7109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>46</v>
       </c>
@@ -10559,7 +10533,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="33" customFormat="1" ht="409.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="33" customFormat="1" ht="409.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>241</v>
       </c>
@@ -10595,70 +10569,70 @@
   </sheetPr>
   <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="76" customWidth="1"/>
-    <col min="3" max="3" width="50.21875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="150" t="s">
+    <row r="1" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="146" t="s">
         <v>352</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="147" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="C6" s="149" t="s">
+      <c r="C6" s="145" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>251</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="2:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="135" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>252</v>
       </c>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>351</v>
       </c>
@@ -10666,7 +10640,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="2:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>247</v>
       </c>
@@ -10674,7 +10648,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>248</v>
       </c>
@@ -10685,7 +10659,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
         <v>343</v>
       </c>
@@ -10696,7 +10670,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="2:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>346</v>
       </c>
@@ -10705,14 +10679,14 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="2:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="148" t="s">
+    <row r="15" spans="2:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="144" t="s">
         <v>355</v>
       </c>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="2:10" ht="131.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="147" t="s">
+    <row r="16" spans="2:10" ht="131.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>350</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -10720,23 +10694,23 @@
       </c>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>349</v>
       </c>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="2:10" ht="346.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="346.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>254</v>
       </c>
@@ -10744,17 +10718,17 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
         <v>258</v>
       </c>

</xml_diff>

<commit_message>
original template from Stephanie
</commit_message>
<xml_diff>
--- a/e8-template.xlsx
+++ b/e8-template.xlsx
@@ -1,35 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephanieInfante\Desktop\temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E734D148-3430-47C5-BD7B-80FFE2188057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="34635" windowHeight="15435" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="13" xr2:uid="{149B6D2C-B18F-46C6-A9A2-8B48A3F23525}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="13" name="1-DoesMyAgencyNeedtoComplete" state="visible" r:id="rId4"/>
-    <sheet sheetId="12" name="2-AboutYourAgency" state="visible" r:id="rId5"/>
-    <sheet sheetId="4" name="3-WhatToComplete" state="visible" r:id="rId6"/>
-    <sheet sheetId="1" name="PR1" state="visible" r:id="rId7"/>
-    <sheet sheetId="14" name="PR2" state="visible" r:id="rId8"/>
-    <sheet sheetId="23" name="PR3" state="visible" r:id="rId9"/>
-    <sheet sheetId="16" name="PR4" state="visible" r:id="rId10"/>
-    <sheet sheetId="17" name="PR5" state="visible" r:id="rId11"/>
-    <sheet sheetId="5" name="FAQ" state="visible" r:id="rId12"/>
-    <sheet sheetId="6" name="AuditAssuranceReportTemplate" state="visible" r:id="rId13"/>
-    <sheet sheetId="8" name="DirectiveTemplate" state="visible" r:id="rId14"/>
-    <sheet sheetId="10" name="SOATemplate" state="visible" r:id="rId15"/>
-    <sheet sheetId="19" name="RiskRegisterTemplate" state="visible" r:id="rId16"/>
-    <sheet sheetId="22" name="Essential8" state="visible" r:id="rId17"/>
-    <sheet sheetId="11" name="SampleAttestation" state="visible" r:id="rId18"/>
-    <sheet sheetId="24" name="data" state="hidden" r:id="rId19"/>
-    <sheet sheetId="3" name="2021Readme" state="hidden" r:id="rId20"/>
+    <sheet name="1-DoesMyAgencyNeedtoComplete" sheetId="13" r:id="rId1"/>
+    <sheet name="2-AboutYourAgency" sheetId="12" r:id="rId2"/>
+    <sheet name="3-WhatToComplete" sheetId="4" r:id="rId3"/>
+    <sheet name="PR1" sheetId="1" r:id="rId4"/>
+    <sheet name="PR2" sheetId="14" r:id="rId5"/>
+    <sheet name="PR3" sheetId="23" r:id="rId6"/>
+    <sheet name="PR4" sheetId="16" r:id="rId7"/>
+    <sheet name="PR5" sheetId="17" r:id="rId8"/>
+    <sheet name="FAQ" sheetId="5" r:id="rId9"/>
+    <sheet name="AuditAssuranceReportTemplate" sheetId="6" r:id="rId10"/>
+    <sheet name="DirectiveTemplate" sheetId="8" r:id="rId11"/>
+    <sheet name="SOATemplate" sheetId="10" r:id="rId12"/>
+    <sheet name="RiskRegisterTemplate" sheetId="19" r:id="rId13"/>
+    <sheet name="Essential8" sheetId="22" r:id="rId14"/>
+    <sheet name="SampleAttestation" sheetId="11" r:id="rId15"/>
+    <sheet name="data" sheetId="24" state="hidden" r:id="rId16"/>
+    <sheet name="2021_Readme" sheetId="3" state="hidden" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'1-DoesMyAgencyNeedtoComplete'!$A1:$I17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'2-AboutYourAgency'!$A2:$C14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'1-DoesMyAgencyNeedtoComplete'!$A$1:$I$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'2-AboutYourAgency'!$A$2:$C$14</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -842,9 +862,6 @@
   </si>
   <si>
     <t>Percentage of systems with regular backups</t>
-  </si>
-  <si>
-    <t>Average of frequency for regular backups</t>
   </si>
   <si>
     <t>Risk treatment for systems/programs without regular backups (evidence may be required)
@@ -1564,6 +1581,9 @@
   </si>
   <si>
     <t>Guideline for conducting Essential Eight reviews</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2139,7 +2159,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
@@ -2382,9 +2402,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -7006,59 +7023,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Readme"/>
-      <sheetName val="Reference"/>
-      <sheetName val="PR1"/>
-      <sheetName val="PR2"/>
-      <sheetName val="PR3"/>
-      <sheetName val="PR4"/>
-      <sheetName val="PR5"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Information Standards"/>
-      <sheetName val="QGEA Policies"/>
-      <sheetName val="Reference"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DF8C5074-499C-744E-971A-9067CECB866C}" name="AboutYou" displayName="AboutYou" ref="A2:C14" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="157">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4E22ACC3-A136-674F-AB2D-C0E12934FA92}" name="Column1" headerRowDxfId="156" headerRowCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{A84757E2-8B75-DD4F-BA7E-51A1C5304BC6}" name="Column2" headerRowDxfId="155"/>
@@ -7070,16 +7036,6 @@
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6164995D-5379-4B4B-AB4D-A1F7140BC99E}" name="PolicyR3e85" displayName="PolicyR3e85" ref="A26:H27" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" headerRowCellStyle="Normal 2" dataCellStyle="20% - Accent2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{CE9FC516-AA87-AA47-BBE7-F770B6728414}" name="PR3-E8.5" dataDxfId="58" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{3669DB3C-1E3A-F141-8792-A74B75841706}" name="Disable untrusted Microsoft Office macros_x000a_Macros are increasingly being used to enable the download of malware.  Adversaries can then access sensitive information, so macros should be secured or disabled" dataDxfId="57" dataCellStyle="Normal 2"/>
@@ -7096,17 +7052,6 @@
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{70ECD7F6-D6AC-3240-8218-56049DE4BA7F}" name="PolicyR3e86" displayName="PolicyR3e86" ref="A29:I30" totalsRowShown="0" headerRowDxfId="50" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ABD558FE-5405-D043-B5BB-041AE84D59F0}" name="PR3-E8.6" dataDxfId="49" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{303CAA2D-9921-9647-B254-DC06DB896724}" name="User application hardening_x000a_Flash, Java and web ads are popular ways to deliver malware to infect computers" dataDxfId="48" dataCellStyle="Normal 2"/>
@@ -7124,16 +7069,6 @@
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{1CBC12C9-0E29-CF4D-A38C-72F34E4C71C3}" name="PolicyR3e87" displayName="PolicyR3e87" ref="A32:H36" totalsRowShown="0" headerRowDxfId="40" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B08649A6-9535-7B4B-9424-F2639303533F}" name="PR3-E8.7" dataDxfId="39" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{D48AFAF8-16EA-C845-AF2F-10692860E891}" name="Multi-factor authentication_x000a_Having multiple levels of authentication makes it harder for adversaries to access your information" dataDxfId="38" dataCellStyle="Normal 2"/>
@@ -7150,23 +7085,12 @@
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{DB2CE024-B531-E342-9F15-E0DD01332C25}" name="PolicyR3e88" displayName="PolicyR3e88" ref="A38:I40" totalsRowShown="0" headerRowDxfId="31" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DA115D66-DA77-C34E-8E5E-B8F3C0C102A3}" name="PR3-E8.8" dataDxfId="30" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{9455DCEF-0621-DE49-A430-2A4CF43CD784}" name="Routine backup of important information_x000a_An organisation can access up to date important information in the event of a security incident" dataDxfId="29" dataCellStyle="Normal 2"/>
     <tableColumn id="3" xr3:uid="{51B2ADE2-B198-5B4A-968A-A4EDBA1A9108}" name="Additional Guidance" dataDxfId="28" dataCellStyle="Normal 2"/>
     <tableColumn id="4" xr3:uid="{D512B5CB-2D4B-824E-8183-8E8EB4D9B912}" name="Percentage of systems with regular backups" dataDxfId="27" dataCellStyle="20% - Accent2"/>
-    <tableColumn id="5" xr3:uid="{49FB7ABB-12D6-CA4B-8FE2-17A97BE874DE}" name="Average of frequency for regular backups" dataDxfId="26" dataCellStyle="Note 2"/>
+    <tableColumn id="5" xr3:uid="{49FB7ABB-12D6-CA4B-8FE2-17A97BE874DE}" name=" " dataDxfId="26" dataCellStyle="Note 2"/>
     <tableColumn id="6" xr3:uid="{6E8FABA8-1A3F-014E-9E5E-0A0D3D2053FA}" name="Risk treatment for systems/programs without regular backups (evidence may be required)_x000a_Please refer to the guideline linked above" dataDxfId="25" dataCellStyle="Note 2"/>
     <tableColumn id="7" xr3:uid="{6FDF44B6-9E44-0D45-8744-514DDA774A8A}" name="Additional Comments (If necessary)" dataDxfId="24" dataCellStyle="Note 2"/>
     <tableColumn id="8" xr3:uid="{0CAFDF03-65F7-624A-930C-DA94F38CE317}" name="Percentage of fleet protected by risk treatment" dataDxfId="23" dataCellStyle="20% - Accent2"/>
@@ -7178,15 +7102,6 @@
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{031FE43E-217C-2649-AC5F-7A44C958A7D1}" name="PolicyR4" displayName="PolicyR4" ref="A1:G4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6E1EDF40-70B6-544B-A986-5E60024AA3D5}" name="#" dataDxfId="16" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{5C238449-1F5D-1D47-AADF-BD451FFA350B}" name="Policy Requirements" dataDxfId="15" dataCellStyle="Normal 2"/>
@@ -7202,13 +7117,6 @@
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{958D11D4-E02A-7043-8E35-69B8DE22E019}" name="PolicyR5" displayName="PolicyR5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E19B852-1D8F-5B41-B909-40400D58B70B}" name="#" dataDxfId="4" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{21CD23DA-3756-6843-894B-9CB4D083C06A}" name="Policy Requirement" dataDxfId="3" dataCellStyle="Normal 2"/>
@@ -7222,18 +7130,6 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92CF42CC-BDE6-4F5E-8166-FF3F2344F966}" name="Table1" displayName="Table1" ref="A1:J4" totalsRowShown="0" headerRowDxfId="153" dataDxfId="152" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="3" xr3:uid="{8A35A1E8-53AD-40CA-8B12-B4E66046888B}" name="How are you providing assurance for your ISMS?_x000a_(Choose one option below)" dataDxfId="151" dataCellStyle="Comma"/>
     <tableColumn id="1" xr3:uid="{4178B884-E6A5-4C91-BB96-D650916A7A5C}" name="I need to provide" dataDxfId="150"/>
@@ -7252,17 +7148,6 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF8D1954-0527-4D54-A6C1-7BED95F1568B}" name="PolicyR1" displayName="PolicyR1" ref="A1:I16" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140" tableBorderDxfId="139">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1D6B8ED-F221-4E0B-871A-CAE3855BB0B1}" name="#" dataDxfId="138" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{1796E134-381D-45F3-B27C-D8F62FA3AA03}" name="Element" dataDxfId="137" dataCellStyle="Normal 2"/>
@@ -7280,15 +7165,6 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2950E7F6-02D7-764D-A273-EA2A6DD44391}" name="PolicyR2" displayName="PolicyR2" ref="A1:G3" totalsRowShown="0" headerRowDxfId="129" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FA59F3E7-505F-2F40-BAFE-861E26F2EE8D}" name="#" dataDxfId="128" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{70BCAEC0-68FC-474D-AF86-1C58BB98A5FB}" name="Policy Requirements" dataDxfId="127" dataCellStyle="Normal 2"/>
@@ -7304,16 +7180,6 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{267DBBEC-EBD9-8047-934C-46C6794C5CA2}" name="PolicyR3" displayName="PolicyR3" ref="A1:H6" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EE3C1643-5589-964D-864E-7B73D51F5975}" name="PR3" dataDxfId="119"/>
     <tableColumn id="2" xr3:uid="{EA5294A1-0FD0-C346-AFD4-64D47D37ACBA}" name="Policy Requirements" dataDxfId="118"/>
@@ -7330,14 +7196,6 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B5BAC64C-6737-4744-A0F0-64FF9F317168}" name="PolicyR3e81" displayName="PolicyR3e81" ref="A10:F12" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0AD3CA88-D8A3-F74D-A507-4590E23BBBF8}" name="PR3- E8.1" dataDxfId="108" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{56037E7E-0FE2-CD44-A74F-89152016EBDC}" name="Application whitelisting_x000a_Use application whitelisting to help prevent malicious software and other unapproved programs from running " dataDxfId="107" dataCellStyle="Normal 2"/>
@@ -7352,19 +7210,6 @@
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4A653377-3B06-4E4A-B9FE-6F7AFAEF870E}" name="PolicyR3e82" displayName="PolicyR3e82" ref="A14:K16" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{38A2B7C7-36B5-0248-9C05-1D30EB7012A6}" name="PR3-E8.2" dataDxfId="99" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{36EC25F1-0F27-8F42-AD9D-0FB4BD449E5E}" name="Patch applications _x000a_Patch applications such as PDF readers, Microsoft Office, Java, Flash Player and web browsers" dataDxfId="98" dataCellStyle="Normal 2"/>
@@ -7384,19 +7229,6 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4C910E91-0772-5946-8CF6-491D3F781DD4}" name="PolicyR3e83" displayName="PolicyR3e83" ref="A18:K21" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87" tableBorderDxfId="86" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B01B4419-95A1-4A4D-A007-B9D68D4BAEEE}" name="PR3- E8.3" dataDxfId="85" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{4084D5B9-3637-E84B-B64B-B744ECD22695}" name="Patch operating systems_x000a_Patch operating system vulnerabilities" dataDxfId="84" dataCellStyle="Normal 2"/>
@@ -7416,19 +7248,6 @@
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{77C3F932-AF6B-2644-9FE3-9CB36F4B1FC3}" name="PolicyR3e84" displayName="PolicyR3e84" ref="A23:K24" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72" headerRowCellStyle="Normal 2">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{66306BC1-EBE7-DC49-AD9D-014EF58F50F2}" name="PR3-E8.4" dataDxfId="71" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{D000608A-BE3C-4C43-BACD-CBF6E4DC7FBC}" name="Minimise users with administrative privileges _x000a_The misuse of administrative privileges is a primary method for attackers to spread inside a target enterprise" dataDxfId="70" dataCellStyle="Normal 2"/>
@@ -7755,160 +7574,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
     </row>
     <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="167" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="168"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="106"/>
-      <c r="B4" s="107"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="170" t="s">
+      <c r="A5" s="169" t="s">
+        <v>304</v>
+      </c>
+      <c r="B5" s="170"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
+      <c r="G5" s="170"/>
+      <c r="H5" s="170"/>
+      <c r="I5" s="171"/>
+    </row>
+    <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="163" t="s">
+        <v>308</v>
+      </c>
+      <c r="B6" s="164"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="164"/>
+      <c r="I6" s="165"/>
+    </row>
+    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="153" t="s">
         <v>305</v>
       </c>
-      <c r="B5" s="171"/>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="171"/>
-      <c r="F5" s="171"/>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="172"/>
-    </row>
-    <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="164" t="s">
-        <v>309</v>
-      </c>
-      <c r="B6" s="165"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="165"/>
-      <c r="F6" s="165"/>
-      <c r="G6" s="165"/>
-      <c r="H6" s="165"/>
-      <c r="I6" s="166"/>
-    </row>
-    <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="154" t="s">
-        <v>306</v>
-      </c>
-      <c r="B7" s="160"/>
-      <c r="C7" s="160"/>
-      <c r="D7" s="160"/>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="161"/>
+      <c r="B7" s="159"/>
+      <c r="C7" s="159"/>
+      <c r="D7" s="159"/>
+      <c r="E7" s="159"/>
+      <c r="F7" s="159"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="159"/>
+      <c r="I7" s="160"/>
     </row>
     <row r="8" spans="1:9" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="152"/>
-      <c r="C8" s="152"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="152"/>
-      <c r="F8" s="152"/>
-      <c r="G8" s="152"/>
-      <c r="H8" s="152"/>
-      <c r="I8" s="153"/>
+      <c r="B8" s="151"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="151"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="151"/>
+      <c r="I8" s="152"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="154" t="s">
+      <c r="A9" s="153" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="155"/>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="155"/>
-      <c r="H9" s="155"/>
-      <c r="I9" s="156"/>
+      <c r="B9" s="154"/>
+      <c r="C9" s="154"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="155"/>
     </row>
     <row r="10" spans="1:9" s="47" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="157" t="s">
+      <c r="A10" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="158"/>
-      <c r="C10" s="158"/>
-      <c r="D10" s="158"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="158"/>
-      <c r="G10" s="158"/>
-      <c r="H10" s="158"/>
-      <c r="I10" s="159"/>
+      <c r="B10" s="157"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="158"/>
     </row>
     <row r="11" spans="1:9" s="47" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="162" t="s">
-        <v>294</v>
-      </c>
-      <c r="B11" s="163"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="163"/>
-      <c r="E11" s="163"/>
-      <c r="F11" s="163"/>
-      <c r="G11" s="163"/>
-      <c r="H11" s="163"/>
-      <c r="I11" s="163"/>
+      <c r="A11" s="161" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11" s="162"/>
+      <c r="C11" s="162"/>
+      <c r="D11" s="162"/>
+      <c r="E11" s="162"/>
+      <c r="F11" s="162"/>
+      <c r="G11" s="162"/>
+      <c r="H11" s="162"/>
+      <c r="I11" s="162"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="108" t="s">
+      <c r="A12" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="150" t="s">
+      <c r="B12" s="108"/>
+      <c r="C12" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="150"/>
-      <c r="E12" s="150"/>
-      <c r="F12" s="150"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="150"/>
-      <c r="I12" s="150"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="149"/>
+      <c r="F12" s="149"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7951,18 +7770,18 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="174" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -8017,23 +7836,23 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="A1" s="174" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -8089,23 +7908,23 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
-        <v>262</v>
-      </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="A1" s="174" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -8161,23 +7980,23 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="A1" s="174" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -8226,7 +8045,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -8236,8 +8055,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
-        <v>331</v>
+      <c r="A1" s="148" t="s">
+        <v>330</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -8247,7 +8066,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -8267,25 +8086,25 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
-        <v>266</v>
-      </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="A1" s="174" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -8347,17 +8166,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -8375,7 +8194,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:I21"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8385,134 +8204,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="175" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="176" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="177" t="s">
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="176" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
-      <c r="F2" s="177"/>
-      <c r="G2" s="177"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="177"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="177" t="s">
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
+      <c r="G3" s="176"/>
+      <c r="H3" s="176"/>
+      <c r="I3" s="176"/>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="176" t="s">
         <v>269</v>
       </c>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="177"/>
-      <c r="G3" s="177"/>
-      <c r="H3" s="177"/>
-      <c r="I3" s="177"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="177" t="s">
+      <c r="B4" s="176"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
+      <c r="H4" s="176"/>
+      <c r="I4" s="176"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="176" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="177" t="s">
+      <c r="B5" s="176"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="176"/>
+      <c r="H5" s="176"/>
+      <c r="I5" s="176"/>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="177" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="178"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="180"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="182"/>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="175" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="179"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="182"/>
-      <c r="H6" s="182"/>
-      <c r="I6" s="183"/>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="176" t="s">
+      <c r="B7" s="175"/>
+      <c r="C7" s="175"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="175"/>
+      <c r="F7" s="175"/>
+      <c r="G7" s="175"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="175"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="176" t="s">
         <v>272</v>
       </c>
-      <c r="B7" s="176"/>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="176"/>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="177" t="s">
+      <c r="B8" s="176"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="176"/>
+      <c r="H8" s="176"/>
+      <c r="I8" s="176"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="175" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="177"/>
-      <c r="F8" s="177"/>
-      <c r="G8" s="177"/>
-      <c r="H8" s="177"/>
-      <c r="I8" s="177"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="176" t="s">
+      <c r="B9" s="175"/>
+      <c r="C9" s="175"/>
+      <c r="D9" s="175"/>
+      <c r="E9" s="175"/>
+      <c r="F9" s="175"/>
+      <c r="G9" s="175"/>
+      <c r="H9" s="175"/>
+      <c r="I9" s="175"/>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="183" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="176"/>
-      <c r="D9" s="176"/>
-      <c r="E9" s="176"/>
-      <c r="F9" s="176"/>
-      <c r="G9" s="176"/>
-      <c r="H9" s="176"/>
-      <c r="I9" s="176"/>
-    </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="184" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="185"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185"/>
-      <c r="F10" s="185"/>
-      <c r="G10" s="185"/>
-      <c r="H10" s="185"/>
-      <c r="I10" s="185"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -8526,43 +8345,43 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="175" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" s="175"/>
+      <c r="C12" s="175"/>
+      <c r="D12" s="175"/>
+      <c r="E12" s="175"/>
+      <c r="F12" s="175"/>
+      <c r="G12" s="175"/>
+      <c r="H12" s="175"/>
+      <c r="I12" s="175"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="187" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="176"/>
-      <c r="F12" s="176"/>
-      <c r="G12" s="176"/>
-      <c r="H12" s="176"/>
-      <c r="I12" s="176"/>
-    </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="188" t="s">
+      <c r="B13" s="187"/>
+      <c r="C13" s="187"/>
+      <c r="D13" s="187"/>
+      <c r="E13" s="187"/>
+      <c r="F13" s="187"/>
+      <c r="G13" s="187"/>
+      <c r="H13" s="187"/>
+      <c r="I13" s="187"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="183" t="s">
         <v>277</v>
       </c>
-      <c r="B13" s="188"/>
-      <c r="C13" s="188"/>
-      <c r="D13" s="188"/>
-      <c r="E13" s="188"/>
-      <c r="F13" s="188"/>
-      <c r="G13" s="188"/>
-      <c r="H13" s="188"/>
-      <c r="I13" s="188"/>
-    </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="184" t="s">
-        <v>278</v>
-      </c>
-      <c r="B14" s="185"/>
-      <c r="C14" s="185"/>
-      <c r="D14" s="185"/>
-      <c r="E14" s="185"/>
-      <c r="F14" s="185"/>
-      <c r="G14" s="185"/>
-      <c r="H14" s="185"/>
-      <c r="I14" s="185"/>
+      <c r="B14" s="184"/>
+      <c r="C14" s="184"/>
+      <c r="D14" s="184"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="184"/>
+      <c r="H14" s="184"/>
+      <c r="I14" s="184"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
@@ -8576,134 +8395,134 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="176" t="s">
+      <c r="A16" s="175" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="175"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="188" t="s">
         <v>279</v>
       </c>
-      <c r="B16" s="176"/>
-      <c r="C16" s="176"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-    </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="189" t="s">
+      <c r="B17" s="188"/>
+      <c r="C17" s="188"/>
+      <c r="D17" s="188"/>
+      <c r="E17" s="188"/>
+      <c r="F17" s="188"/>
+      <c r="G17" s="188"/>
+      <c r="H17" s="188"/>
+      <c r="I17" s="188"/>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="189" t="s">
         <v>280</v>
       </c>
-      <c r="B17" s="189"/>
-      <c r="C17" s="189"/>
-      <c r="D17" s="189"/>
-      <c r="E17" s="189"/>
-      <c r="F17" s="189"/>
-      <c r="G17" s="189"/>
-      <c r="H17" s="189"/>
-      <c r="I17" s="189"/>
-    </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="190" t="s">
+      <c r="B18" s="190"/>
+      <c r="C18" s="190"/>
+      <c r="D18" s="190"/>
+      <c r="E18" s="190"/>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="190"/>
+      <c r="I18" s="190"/>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="191" t="s">
         <v>281</v>
       </c>
-      <c r="B18" s="191"/>
-      <c r="C18" s="191"/>
-      <c r="D18" s="191"/>
-      <c r="E18" s="191"/>
-      <c r="F18" s="191"/>
-      <c r="G18" s="191"/>
-      <c r="H18" s="191"/>
-      <c r="I18" s="191"/>
-    </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="192" t="s">
+      <c r="B19" s="191"/>
+      <c r="C19" s="191"/>
+      <c r="D19" s="191"/>
+      <c r="E19" s="191"/>
+      <c r="F19" s="191"/>
+      <c r="G19" s="191"/>
+      <c r="H19" s="191"/>
+      <c r="I19" s="191"/>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="192" t="s">
         <v>282</v>
       </c>
-      <c r="B19" s="192"/>
-      <c r="C19" s="192"/>
-      <c r="D19" s="192"/>
-      <c r="E19" s="192"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="192"/>
-      <c r="I19" s="192"/>
-    </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="193" t="s">
+      <c r="B20" s="192"/>
+      <c r="C20" s="192"/>
+      <c r="D20" s="192"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
+      <c r="G20" s="192"/>
+      <c r="H20" s="192"/>
+      <c r="I20" s="192"/>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="176" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="193"/>
-      <c r="C20" s="193"/>
-      <c r="D20" s="193"/>
-      <c r="E20" s="193"/>
-      <c r="F20" s="193"/>
-      <c r="G20" s="193"/>
-      <c r="H20" s="193"/>
-      <c r="I20" s="193"/>
-    </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="177" t="s">
+      <c r="B21" s="176"/>
+      <c r="C21" s="176"/>
+      <c r="D21" s="176"/>
+      <c r="E21" s="176"/>
+      <c r="F21" s="176"/>
+      <c r="G21" s="176"/>
+      <c r="H21" s="176"/>
+      <c r="I21" s="176"/>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="175" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="177"/>
-      <c r="C21" s="177"/>
-      <c r="D21" s="177"/>
-      <c r="E21" s="177"/>
-      <c r="F21" s="177"/>
-      <c r="G21" s="177"/>
-      <c r="H21" s="177"/>
-      <c r="I21" s="177"/>
-    </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="176" t="s">
+      <c r="B22" s="175"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="175"/>
+      <c r="E22" s="175"/>
+      <c r="F22" s="175"/>
+      <c r="G22" s="175"/>
+      <c r="H22" s="175"/>
+      <c r="I22" s="175"/>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="193" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="176"/>
-      <c r="C22" s="176"/>
-      <c r="D22" s="176"/>
-      <c r="E22" s="176"/>
-      <c r="F22" s="176"/>
-      <c r="G22" s="176"/>
-      <c r="H22" s="176"/>
-      <c r="I22" s="176"/>
-    </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="194" t="s">
+      <c r="B23" s="193"/>
+      <c r="C23" s="193"/>
+      <c r="D23" s="193"/>
+      <c r="E23" s="193"/>
+      <c r="F23" s="193"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="175" t="s">
         <v>286</v>
       </c>
-      <c r="B23" s="194"/>
-      <c r="C23" s="194"/>
-      <c r="D23" s="194"/>
-      <c r="E23" s="194"/>
-      <c r="F23" s="194"/>
-      <c r="G23" s="194"/>
-      <c r="H23" s="194"/>
-      <c r="I23" s="194"/>
-    </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="176" t="s">
-        <v>287</v>
-      </c>
-      <c r="B24" s="176"/>
-      <c r="C24" s="176"/>
-      <c r="D24" s="176"/>
-      <c r="E24" s="176"/>
-      <c r="F24" s="176"/>
-      <c r="G24" s="176"/>
-      <c r="H24" s="176"/>
-      <c r="I24" s="176"/>
+      <c r="B24" s="175"/>
+      <c r="C24" s="175"/>
+      <c r="D24" s="175"/>
+      <c r="E24" s="175"/>
+      <c r="F24" s="175"/>
+      <c r="G24" s="175"/>
+      <c r="H24" s="175"/>
+      <c r="I24" s="175"/>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="186" t="s">
+      <c r="A25" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="187"/>
-      <c r="C25" s="187"/>
-      <c r="D25" s="187"/>
-      <c r="E25" s="187"/>
-      <c r="F25" s="187"/>
-      <c r="G25" s="187"/>
-      <c r="H25" s="187"/>
-      <c r="I25" s="187"/>
+      <c r="B25" s="186"/>
+      <c r="C25" s="186"/>
+      <c r="D25" s="186"/>
+      <c r="E25" s="186"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="186"/>
+      <c r="H25" s="186"/>
+      <c r="I25" s="186"/>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
@@ -8781,14 +8600,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="121" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="122" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="25" t="s">
@@ -8797,103 +8616,103 @@
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="123" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="121"/>
+      <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:3" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="124" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="C5" s="131" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="132" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="122" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" s="132" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="125" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="123" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="C6" s="133" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="126" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>313</v>
-      </c>
-    </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="127" t="s">
+      <c r="A8" s="126" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="26">
         <v>468463789</v>
       </c>
-      <c r="C8" s="121"/>
+      <c r="C8" s="120"/>
     </row>
     <row r="9" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="128"/>
-      <c r="B9" s="111"/>
+      <c r="A9" s="127"/>
+      <c r="B9" s="110"/>
     </row>
     <row r="10" spans="1:3" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="128" t="s">
+      <c r="A10" s="127" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="21">
         <v>0</v>
       </c>
-      <c r="C10" s="130" t="s">
-        <v>315</v>
+      <c r="C10" s="129" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="128" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="29">
         <v>0</v>
       </c>
-      <c r="C11" s="134" t="s">
-        <v>316</v>
+      <c r="C11" s="133" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="130" t="s">
+      <c r="A12" s="129" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="135"/>
+      <c r="C12" s="134"/>
     </row>
     <row r="13" spans="1:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
+      <c r="A13" s="130"/>
       <c r="B13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="136"/>
+      <c r="C13" s="135"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="139"/>
+      <c r="C14" s="138"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8920,7 +8739,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8935,28 +8754,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="102" t="s">
         <v>29</v>
       </c>
       <c r="I1" s="76" t="s">
@@ -8968,10 +8787,10 @@
     </row>
     <row r="2" spans="1:10" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>32</v>
@@ -8983,7 +8802,7 @@
         <v>33</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>34</v>
@@ -8992,18 +8811,18 @@
         <v>35</v>
       </c>
       <c r="I2" s="77" t="s">
-        <v>295</v>
-      </c>
-      <c r="J2" s="104" t="s">
+        <v>294</v>
+      </c>
+      <c r="J2" s="103" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>37</v>
@@ -9015,7 +8834,7 @@
         <v>38</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>39</v>
@@ -9024,15 +8843,15 @@
         <v>35</v>
       </c>
       <c r="I3" s="77" t="s">
-        <v>297</v>
-      </c>
-      <c r="J3" s="104" t="s">
+        <v>296</v>
+      </c>
+      <c r="J3" s="103" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="199.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>41</v>
@@ -9047,7 +8866,7 @@
         <v>38</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G4" s="35" t="s">
         <v>44</v>
@@ -9056,9 +8875,9 @@
         <v>35</v>
       </c>
       <c r="I4" s="77" t="s">
-        <v>296</v>
-      </c>
-      <c r="J4" s="104" t="s">
+        <v>295</v>
+      </c>
+      <c r="J4" s="103" t="s">
         <v>45</v>
       </c>
     </row>
@@ -9080,7 +8899,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9096,36 +8915,36 @@
     <col min="10" max="16384" width="8.7109375" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:9" s="101" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="99" t="s">
-        <v>322</v>
-      </c>
-      <c r="F1" s="99" t="s">
-        <v>319</v>
-      </c>
-      <c r="G1" s="100" t="s">
+      <c r="E1" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="F1" s="98" t="s">
+        <v>318</v>
+      </c>
+      <c r="G1" s="99" t="s">
+        <v>320</v>
+      </c>
+      <c r="H1" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="100" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="101" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
         <v>53</v>
       </c>
@@ -9134,17 +8953,17 @@
       </c>
       <c r="C2" s="83"/>
       <c r="D2" s="83" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E2" s="85" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F2" s="85"/>
       <c r="G2" s="86"/>
-      <c r="H2" s="113" t="s">
+      <c r="H2" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="112"/>
+      <c r="I2" s="111"/>
     </row>
     <row r="3" spans="1:9" ht="266.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="82" t="s">
@@ -9160,14 +8979,14 @@
         <v>59</v>
       </c>
       <c r="E3" s="85" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F3" s="85" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G3" s="86"/>
-      <c r="H3" s="141" t="s">
-        <v>339</v>
+      <c r="H3" s="140" t="s">
+        <v>338</v>
       </c>
       <c r="I3" s="59" t="s">
         <v>61</v>
@@ -9187,7 +9006,7 @@
         <v>64</v>
       </c>
       <c r="E4" s="85" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F4" s="85"/>
       <c r="G4" s="86"/>
@@ -9214,8 +9033,8 @@
       <c r="E5" s="85"/>
       <c r="F5" s="85"/>
       <c r="G5" s="86"/>
-      <c r="H5" s="141" t="s">
-        <v>339</v>
+      <c r="H5" s="140" t="s">
+        <v>338</v>
       </c>
       <c r="I5" s="59" t="s">
         <v>69</v>
@@ -9237,8 +9056,8 @@
       <c r="E6" s="85"/>
       <c r="F6" s="85"/>
       <c r="G6" s="86"/>
-      <c r="H6" s="141" t="s">
-        <v>339</v>
+      <c r="H6" s="140" t="s">
+        <v>338</v>
       </c>
       <c r="I6" s="59" t="s">
         <v>73</v>
@@ -9260,7 +9079,7 @@
       <c r="E7" s="85"/>
       <c r="F7" s="85"/>
       <c r="G7" s="86"/>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="142" t="s">
         <v>78</v>
       </c>
       <c r="I7" s="59" t="s">
@@ -9283,8 +9102,8 @@
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
       <c r="G8" s="86"/>
-      <c r="H8" s="143" t="s">
-        <v>341</v>
+      <c r="H8" s="142" t="s">
+        <v>340</v>
       </c>
       <c r="I8" s="59" t="s">
         <v>83</v>
@@ -9306,8 +9125,8 @@
       <c r="E9" s="85"/>
       <c r="F9" s="85"/>
       <c r="G9" s="86"/>
-      <c r="H9" s="143" t="s">
-        <v>341</v>
+      <c r="H9" s="142" t="s">
+        <v>340</v>
       </c>
       <c r="I9" s="59" t="s">
         <v>87</v>
@@ -9329,7 +9148,7 @@
       <c r="E10" s="85"/>
       <c r="F10" s="85"/>
       <c r="G10" s="86"/>
-      <c r="H10" s="91"/>
+      <c r="H10" s="90"/>
       <c r="I10" s="59" t="s">
         <v>92</v>
       </c>
@@ -9350,7 +9169,7 @@
       <c r="E11" s="85"/>
       <c r="F11" s="85"/>
       <c r="G11" s="86"/>
-      <c r="H11" s="91"/>
+      <c r="H11" s="90"/>
       <c r="I11" s="59" t="s">
         <v>96</v>
       </c>
@@ -9371,7 +9190,7 @@
       <c r="E12" s="85"/>
       <c r="F12" s="85"/>
       <c r="G12" s="86"/>
-      <c r="H12" s="91"/>
+      <c r="H12" s="90"/>
       <c r="I12" s="59" t="s">
         <v>100</v>
       </c>
@@ -9392,8 +9211,8 @@
       <c r="E13" s="85"/>
       <c r="F13" s="85"/>
       <c r="G13" s="86"/>
-      <c r="H13" s="142" t="s">
-        <v>340</v>
+      <c r="H13" s="141" t="s">
+        <v>339</v>
       </c>
       <c r="I13" s="59" t="s">
         <v>104</v>
@@ -9415,8 +9234,8 @@
       <c r="E14" s="85"/>
       <c r="F14" s="85"/>
       <c r="G14" s="86"/>
-      <c r="H14" s="142" t="s">
-        <v>340</v>
+      <c r="H14" s="141" t="s">
+        <v>339</v>
       </c>
       <c r="I14" s="59" t="s">
         <v>108</v>
@@ -9438,28 +9257,28 @@
       <c r="E15" s="85"/>
       <c r="F15" s="85"/>
       <c r="G15" s="86"/>
-      <c r="H15" s="91"/>
+      <c r="H15" s="90"/>
       <c r="I15" s="59" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="94" t="s">
+      <c r="D16" s="93" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="94"/>
       <c r="I16" s="59" t="s">
         <v>117</v>
       </c>
@@ -9471,9 +9290,9 @@
     <hyperlink ref="H4" location="DirectiveTemplate!A1" display="DirectiveTemplate!A1" xr:uid="{F76C857D-D742-48D3-92E9-B28006E73922}"/>
     <hyperlink ref="H5" location="DirectiveTemplate!A1" display="DirectiveTemplate" xr:uid="{534CB86D-5334-4ACC-8304-A357134FD280}"/>
     <hyperlink ref="H6" location="DirectiveTemplate!A1" display="DirectiveTemplate" xr:uid="{80987C41-B12B-40C8-A190-951B3660F850}"/>
-    <hyperlink ref="H7" location="'SOA Template'!A1" display="'SOA Template'!A1" xr:uid="{7C575122-2C62-4A75-B747-F3EFB2EE317B}"/>
-    <hyperlink ref="H8" location="'SOA Template'!A1" display="SOA Template" xr:uid="{E9E791FA-3B29-4745-ABC3-6BBBF506F9A0}"/>
-    <hyperlink ref="H9" location="'SOA Template'!A1" display="SOA Template" xr:uid="{1D81827D-AAC5-4384-A4DA-D4263BAC223F}"/>
+    <hyperlink ref="H7" location="SOATemplate!A1" display="SOA Template'!A1" xr:uid="{7C575122-2C62-4A75-B747-F3EFB2EE317B}"/>
+    <hyperlink ref="H8" location="SOATemplate!A1" display="SOA Template" xr:uid="{E9E791FA-3B29-4745-ABC3-6BBBF506F9A0}"/>
+    <hyperlink ref="H9" location="SOATemplate!A1" display="SOA Template" xr:uid="{1D81827D-AAC5-4384-A4DA-D4263BAC223F}"/>
     <hyperlink ref="H13" location="RiskRegisterTemplate!A1" display="RiskRegisterTemplate" xr:uid="{08A29202-ED02-4848-8D0A-12AFC5686102}"/>
     <hyperlink ref="H14" location="RiskRegisterTemplate!A1" display="RiskRegisterTemplate" xr:uid="{8D5295B6-0B4C-429D-8528-6DC718811C37}"/>
     <hyperlink ref="H2" location="'AuditAssuranceReportTemplate'!A1" display="Audit Assurance Report Template" xr:uid="{456CC15D-B489-41C9-B213-E1E0397205BF}"/>
@@ -9521,13 +9340,13 @@
         <v>49</v>
       </c>
       <c r="D1" s="78" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" s="78" t="s">
         <v>323</v>
-      </c>
-      <c r="E1" s="78" t="s">
-        <v>319</v>
-      </c>
-      <c r="F1" s="78" t="s">
-        <v>324</v>
       </c>
       <c r="G1" s="79" t="s">
         <v>52</v>
@@ -9542,11 +9361,11 @@
       </c>
       <c r="C2" s="83"/>
       <c r="D2" s="83" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E2" s="85"/>
       <c r="F2" s="86"/>
-      <c r="G2" s="113" t="s">
+      <c r="G2" s="112" t="s">
         <v>55</v>
       </c>
     </row>
@@ -9560,15 +9379,15 @@
       <c r="C3" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="120" t="s">
-        <v>357</v>
-      </c>
-      <c r="E3" s="120" t="s">
+      <c r="D3" s="119" t="s">
         <v>356</v>
+      </c>
+      <c r="E3" s="119" t="s">
+        <v>355</v>
       </c>
       <c r="F3" s="77"/>
       <c r="G3" s="80" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9578,9 +9397,9 @@
       <c r="D8" s="83"/>
       <c r="E8" s="85"/>
       <c r="F8" s="86"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="102"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="101"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9588,7 +9407,7 @@
     <hyperlink ref="G2" location="'AuditAssuranceReportTemplate'!A1" display="Audit Assurance Report Template" xr:uid="{83E0E6DE-13A8-4257-A5BF-19FB1696852D}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -9602,8 +9421,8 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="E29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I38" sqref="E38:I38"/>
+    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9636,10 +9455,10 @@
         <v>123</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G1" s="49" t="s">
         <v>51</v>
@@ -9656,12 +9475,12 @@
         <v>54</v>
       </c>
       <c r="C2" s="83" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D2" s="83"/>
       <c r="E2" s="85"/>
       <c r="F2" s="86"/>
-      <c r="G2" s="113"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="12" t="s">
         <v>55</v>
       </c>
@@ -9673,12 +9492,12 @@
       <c r="B3" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="100" t="s">
         <v>125</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G3" s="73"/>
       <c r="H3" s="73"/>
@@ -9691,14 +9510,14 @@
         <v>127</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="74"/>
       <c r="E4" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H4" s="48" t="s">
         <v>128</v>
@@ -9712,7 +9531,7 @@
         <v>130</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D5" s="74"/>
       <c r="H5" s="48" t="s">
@@ -9727,7 +9546,7 @@
         <v>133</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D6" s="74"/>
       <c r="H6" s="48" t="s">
@@ -9735,34 +9554,34 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="110"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
     </row>
     <row r="8" spans="1:11" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="148" t="s">
-        <v>358</v>
+      <c r="B8" s="147" t="s">
+        <v>357</v>
       </c>
       <c r="C8" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>337</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>338</v>
       </c>
       <c r="E8" s="48"/>
       <c r="H8" s="50"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="73"/>
-      <c r="B9" s="105"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
       <c r="E9" s="12"/>
@@ -10148,13 +9967,13 @@
         <v>178</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E26" s="52" t="s">
         <v>190</v>
       </c>
       <c r="F26" s="52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G26" s="52" t="s">
         <v>191</v>
@@ -10163,10 +9982,10 @@
         <v>183</v>
       </c>
       <c r="I26" s="53"/>
-      <c r="J26" s="174" t="s">
+      <c r="J26" s="173" t="s">
         <v>155</v>
       </c>
-      <c r="K26" s="174"/>
+      <c r="K26" s="173"/>
     </row>
     <row r="27" spans="1:11" ht="91.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54" t="s">
@@ -10190,8 +10009,8 @@
       </c>
       <c r="H27" s="56"/>
       <c r="I27" s="53"/>
-      <c r="J27" s="173"/>
-      <c r="K27" s="173"/>
+      <c r="J27" s="172"/>
+      <c r="K27" s="172"/>
     </row>
     <row r="28" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="60"/>
@@ -10287,14 +10106,14 @@
       <c r="E32" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F32" s="140" t="s">
-        <v>336</v>
+      <c r="F32" s="139" t="s">
+        <v>335</v>
       </c>
       <c r="G32" s="52" t="s">
         <v>210</v>
       </c>
       <c r="H32" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I32" s="52"/>
     </row>
@@ -10417,16 +10236,16 @@
         <v>225</v>
       </c>
       <c r="E38" s="52" t="s">
+        <v>363</v>
+      </c>
+      <c r="F38" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="52" t="s">
+      <c r="G38" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="G38" s="52" t="s">
-        <v>228</v>
-      </c>
       <c r="H38" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I38" s="58" t="s">
         <v>210</v>
@@ -10434,13 +10253,13 @@
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="B39" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="C39" s="55" t="s">
         <v>230</v>
-      </c>
-      <c r="C39" s="55" t="s">
-        <v>231</v>
       </c>
       <c r="D39" s="56">
         <v>0</v>
@@ -10457,13 +10276,13 @@
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="55" t="s">
         <v>232</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="C40" s="55" t="s">
         <v>233</v>
-      </c>
-      <c r="C40" s="55" t="s">
-        <v>234</v>
       </c>
       <c r="D40" s="56">
         <v>0</v>
@@ -10545,7 +10364,7 @@
         <v>50</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F1" s="41" t="s">
         <v>51</v>
@@ -10556,48 +10375,48 @@
     </row>
     <row r="2" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="87" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B2" s="88" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="83"/>
       <c r="D2" s="83" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E2" s="85"/>
       <c r="F2" s="86"/>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="113" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="337.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="C3" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="D3" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="E3" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>238</v>
-      </c>
       <c r="F3" s="44"/>
-      <c r="G3" s="115"/>
+      <c r="G3" s="114"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="116"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="32"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="115"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="114"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10638,33 +10457,33 @@
         <v>46</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C1" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="33" customFormat="1" ht="409.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="C2" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="45" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>327</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -10686,7 +10505,7 @@
   </sheetPr>
   <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -10697,61 +10516,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="146" t="s">
-        <v>352</v>
-      </c>
-      <c r="C1" s="147" t="s">
-        <v>244</v>
+      <c r="B1" s="145" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="146" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="C6" s="145" t="s">
+        <v>353</v>
+      </c>
+      <c r="C6" s="144" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C7" s="14"/>
     </row>
     <row r="8" spans="2:10" ht="135" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="14"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -10759,7 +10578,7 @@
     </row>
     <row r="11" spans="2:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -10767,10 +10586,10 @@
     </row>
     <row r="12" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>248</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>249</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -10778,10 +10597,10 @@
     </row>
     <row r="13" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -10789,7 +10608,7 @@
     </row>
     <row r="14" spans="2:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="10"/>
@@ -10797,57 +10616,57 @@
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="144" t="s">
-        <v>355</v>
+      <c r="B15" s="143" t="s">
+        <v>354</v>
       </c>
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="2:10" ht="131.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="2:10" ht="346.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>254</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -11147,16 +10966,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDB849-2D35-4D47-8357-5A24A389B99C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2ea85696-5d49-4719-8940-b51507ccf115"/>
     <ds:schemaRef ds:uri="474a08bd-ae9f-4ab7-ab72-cad3c4647737"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="2ea85696-5d49-4719-8940-b51507ccf115"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>